<commit_message>
Added tests for Citations, Removed page-with-metatag-data.xlsx, Added more data to searchenginerestrictions_data.xlsx
</commit_message>
<xml_diff>
--- a/test-data/citations-data.xlsx
+++ b/test-data/citations-data.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BB1798-F645-41E0-87A9-A1F9514B1C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB4F7AF-6C93-49A4-A32E-957E2D827E5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_citations" sheetId="1" r:id="rId1"/>
+    <sheet name="pages_without_citations" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
   <si>
     <t>path</t>
   </si>
@@ -46,9 +47,6 @@
     <t>/types/breast/reconstruction-fact-sheet</t>
   </si>
   <si>
-    <t>/espanol/cancer/sobrellevar/sentimientos/hoja-informativa-estres</t>
-  </si>
-  <si>
     <t>expectedHeaderText</t>
   </si>
   <si>
@@ -73,17 +71,123 @@
     <t>/news-events/cancer-currents-blog/2019/transition-lowy-nci-acting-director</t>
   </si>
   <si>
-    <t>Blogs</t>
+    <t>expectedPubMedUrl</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/21460648</t>
+  </si>
+  <si>
+    <t>/news-events/cancer-currents-blog</t>
+  </si>
+  <si>
+    <t>Blog Series</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/temas-y-relatos-blog</t>
+  </si>
+  <si>
+    <t>Blog Post</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/chanock-stephen</t>
+  </si>
+  <si>
+    <t>Biography</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/dfharvard</t>
+  </si>
+  <si>
+    <t>Cancer Center</t>
+  </si>
+  <si>
+    <t>/types/breast/research</t>
+  </si>
+  <si>
+    <t>Cancer Research List Page</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/seno/investigacion</t>
+  </si>
+  <si>
+    <t>/types/breast</t>
+  </si>
+  <si>
+    <t>Cancer Type Home Page</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/seno</t>
+  </si>
+  <si>
+    <t>/types/breast/hp</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings/relaxation/2019-investigators-site</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Home &amp; Landing</t>
+  </si>
+  <si>
+    <t>/about-cancer</t>
+  </si>
+  <si>
+    <t>/espanol/cancer</t>
+  </si>
+  <si>
+    <t>/news-events/press-releases/2018</t>
+  </si>
+  <si>
+    <t>Mini Landing Page</t>
+  </si>
+  <si>
+    <t>/espanol/noticias/comunicados-de-prensa/2018</t>
+  </si>
+  <si>
+    <t>/espanol/efectos-secundarios</t>
+  </si>
+  <si>
+    <t>/about-nci/organization/screen-to-save-infographic</t>
+  </si>
+  <si>
+    <t>Infographic</t>
+  </si>
+  <si>
+    <t>/espanol/infografia-nci</t>
+  </si>
+  <si>
+    <t>/research/progress/discovery/gutcheck-intro-video</t>
+  </si>
+  <si>
+    <t>Video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,13 +210,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,21 +513,24 @@
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -430,10 +541,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -444,12 +558,15 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -458,53 +575,286 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{629353FB-1AFB-4A79-8BFB-A68243A0B030}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693BD2D3-6348-48F5-98A9-0A4DB7F6917A}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>